<commit_message>
feat: empty row for markdowns
</commit_message>
<xml_diff>
--- a/tests/data_up_to_S2022T04/Torneo S2022T01 para publicar.xlsx
+++ b/tests/data_up_to_S2022T04/Torneo S2022T01 para publicar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Nivel de Juego Torneo 01 2022" sheetId="1" state="visible" r:id="rId2"/>
@@ -1574,13 +1574,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A29" activeCellId="1" sqref="21:21 A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1802,35 +1802,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>14</v>
-      </c>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1838,16 +1831,13 @@
         <v>36</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1855,16 +1845,16 @@
         <v>36</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,13 +1862,16 @@
         <v>36</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1886,16 +1879,13 @@
         <v>36</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,10 +1893,10 @@
         <v>36</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>19</v>
@@ -1920,16 +1910,16 @@
         <v>36</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1937,16 +1927,16 @@
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1954,13 +1944,16 @@
         <v>36</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1968,16 +1961,13 @@
         <v>36</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1985,10 +1975,10 @@
         <v>36</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>5</v>
@@ -2002,16 +1992,16 @@
         <v>36</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2019,61 +2009,51 @@
         <v>36</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>73</v>
-      </c>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>5</v>
@@ -2087,16 +2067,16 @@
         <v>68</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2104,13 +2084,13 @@
         <v>68</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>14</v>
@@ -2121,16 +2101,16 @@
         <v>68</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,10 +2118,16 @@
         <v>68</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2149,16 +2135,16 @@
         <v>68</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2166,13 +2152,10 @@
         <v>68</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2180,16 +2163,16 @@
         <v>68</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2197,10 +2180,13 @@
         <v>68</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2208,10 +2194,10 @@
         <v>68</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>19</v>
@@ -2225,16 +2211,10 @@
         <v>68</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,10 +2222,16 @@
         <v>68</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,16 +2239,16 @@
         <v>68</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2270,16 +2256,10 @@
         <v>68</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2287,10 +2267,16 @@
         <v>68</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2298,16 +2284,16 @@
         <v>68</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2315,10 +2301,10 @@
         <v>68</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2326,10 +2312,16 @@
         <v>68</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2337,16 +2329,10 @@
         <v>68</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2354,10 +2340,10 @@
         <v>68</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2365,15 +2351,43 @@
         <v>68</v>
       </c>
       <c r="B51" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D53" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E53" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2401,10 +2415,10 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+      <selection pane="topLeft" activeCell="K4" activeCellId="1" sqref="21:21 K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="6" t="s">
@@ -2515,13 +2529,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A36" activeCellId="1" sqref="21:21 A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2868,47 +2882,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E16" s="4" t="n">
-        <v>-3</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="4" t="n">
-        <v>0.5</v>
-      </c>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D17" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" s="4" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>127</v>
@@ -2922,19 +2920,19 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E18" s="4" t="n">
-        <v>-16</v>
+        <v>-1</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>127</v>
@@ -2943,24 +2941,24 @@
         <v>36</v>
       </c>
       <c r="H18" s="4" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D19" s="4" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E19" s="4" t="n">
-        <v>-4</v>
+        <v>-16</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>127</v>
@@ -2977,19 +2975,19 @@
         <v>152</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E20" s="4" t="n">
-        <v>-14</v>
+        <v>-4</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>36</v>
@@ -3000,22 +2998,22 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D21" s="4" t="n">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E21" s="4" t="n">
-        <v>-36</v>
+        <v>-14</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>36</v>
@@ -3026,22 +3024,22 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D22" s="4" t="n">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="E22" s="4" t="n">
-        <v>-6</v>
+        <v>-36</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>36</v>
@@ -3052,19 +3050,19 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D23" s="4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E23" s="4" t="n">
-        <v>-10</v>
+        <v>-6</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>136</v>
@@ -3078,28 +3076,28 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D24" s="4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E24" s="4" t="n">
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>36</v>
       </c>
       <c r="H24" s="4" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3107,16 +3105,16 @@
         <v>150</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D25" s="4" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E25" s="4" t="n">
-        <v>-14</v>
+        <v>-2</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>139</v>
@@ -3125,24 +3123,24 @@
         <v>36</v>
       </c>
       <c r="H25" s="4" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D26" s="4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E26" s="4" t="n">
-        <v>-1</v>
+        <v>-14</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>139</v>
@@ -3151,7 +3149,7 @@
         <v>36</v>
       </c>
       <c r="H26" s="4" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3159,16 +3157,16 @@
         <v>125</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D27" s="4" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E27" s="4" t="n">
-        <v>-8</v>
+        <v>-1</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>139</v>
@@ -3177,7 +3175,7 @@
         <v>36</v>
       </c>
       <c r="H27" s="4" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3185,10 +3183,10 @@
         <v>125</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D28" s="4" t="n">
         <v>8</v>
@@ -3208,19 +3206,19 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D29" s="4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E29" s="4" t="n">
-        <v>-2</v>
+        <v>-8</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>139</v>
@@ -3229,7 +3227,7 @@
         <v>36</v>
       </c>
       <c r="H29" s="4" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3237,16 +3235,16 @@
         <v>146</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D30" s="4" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E30" s="4" t="n">
-        <v>-8</v>
+        <v>-2</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>139</v>
@@ -3255,24 +3253,24 @@
         <v>36</v>
       </c>
       <c r="H30" s="4" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D31" s="4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E31" s="4" t="n">
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>139</v>
@@ -3286,19 +3284,19 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D32" s="4" t="n">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="E32" s="4" t="n">
-        <v>-63</v>
+        <v>-6</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>139</v>
@@ -3307,24 +3305,24 @@
         <v>36</v>
       </c>
       <c r="H32" s="4" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D33" s="4" t="n">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="E33" s="4" t="n">
-        <v>-2</v>
+        <v>-63</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>139</v>
@@ -3333,24 +3331,24 @@
         <v>36</v>
       </c>
       <c r="H33" s="4" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>147</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D34" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" s="4" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>139</v>
@@ -3367,16 +3365,16 @@
         <v>152</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D35" s="4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E35" s="4" t="n">
-        <v>-6</v>
+        <v>-1</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>139</v>
@@ -3385,18 +3383,18 @@
         <v>36</v>
       </c>
       <c r="H35" s="4" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D36" s="4" t="n">
         <v>6</v>
@@ -3405,56 +3403,40 @@
         <v>-6</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="H36" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D37" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E37" s="4" t="n">
-        <v>-6</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H37" s="4" t="n">
-        <v>1</v>
-      </c>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D38" s="4" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E38" s="4" t="n">
-        <v>-8</v>
+        <v>-6</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>127</v>
@@ -3468,19 +3450,19 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D39" s="4" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E39" s="4" t="n">
-        <v>-16</v>
+        <v>-6</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>127</v>
@@ -3497,19 +3479,19 @@
         <v>144</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D40" s="4" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E40" s="4" t="n">
-        <v>-18</v>
+        <v>-8</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>68</v>
@@ -3520,22 +3502,22 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D41" s="4" t="n">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E41" s="4" t="n">
-        <v>-26</v>
+        <v>-16</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>68</v>
@@ -3546,22 +3528,22 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>173</v>
-      </c>
       <c r="C42" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D42" s="4" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E42" s="4" t="n">
-        <v>-26</v>
+        <v>-18</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>68</v>
@@ -3572,22 +3554,22 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D43" s="4" t="n">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E43" s="4" t="n">
-        <v>-8</v>
+        <v>-26</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>68</v>
@@ -3598,22 +3580,22 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="C44" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D44" s="4" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E44" s="4" t="n">
-        <v>-6</v>
+        <v>-26</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>68</v>
@@ -3624,22 +3606,22 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D45" s="4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E45" s="4" t="n">
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>68</v>
@@ -3650,19 +3632,19 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>189</v>
+        <v>147</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D46" s="4" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E46" s="4" t="n">
-        <v>-8</v>
+        <v>-6</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>139</v>
@@ -3676,19 +3658,19 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D47" s="4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E47" s="4" t="n">
-        <v>-10</v>
+        <v>-6</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>139</v>
@@ -3702,19 +3684,19 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D48" s="4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E48" s="4" t="n">
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>139</v>
@@ -3728,19 +3710,19 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D49" s="4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E49" s="4" t="n">
-        <v>-8</v>
+        <v>-10</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>139</v>
@@ -3754,19 +3736,19 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D50" s="4" t="n">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="E50" s="4" t="n">
-        <v>-42</v>
+        <v>-6</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>139</v>
@@ -3780,19 +3762,19 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D51" s="4" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E51" s="4" t="n">
-        <v>-14</v>
+        <v>-8</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>139</v>
@@ -3809,16 +3791,16 @@
         <v>180</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D52" s="4" t="n">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E52" s="4" t="n">
-        <v>-26</v>
+        <v>-42</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>139</v>
@@ -3832,19 +3814,19 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D53" s="4" t="n">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E53" s="4" t="n">
-        <v>-30</v>
+        <v>-14</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>139</v>
@@ -3858,19 +3840,19 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>147</v>
+        <v>180</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D54" s="4" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E54" s="4" t="n">
-        <v>-22</v>
+        <v>-26</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>139</v>
@@ -3884,19 +3866,19 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D55" s="4" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E55" s="4" t="n">
-        <v>-12</v>
+        <v>-30</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>139</v>
@@ -3905,6 +3887,58 @@
         <v>68</v>
       </c>
       <c r="H55" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D56" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="E56" s="4" t="n">
+        <v>-22</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H56" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D57" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="E57" s="4" t="n">
+        <v>-12</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H57" s="4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3929,13 +3963,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A36" activeCellId="1" sqref="21:21 A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4210,38 +4244,26 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>36</v>
-      </c>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4" t="n">
         <v>3</v>
-      </c>
-      <c r="D17" s="4" t="n">
-        <v>0</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>127</v>
@@ -4252,10 +4274,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>3</v>
@@ -4272,16 +4294,16 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="C19" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" s="4" t="n">
         <v>0</v>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>3</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>127</v>
@@ -4292,7 +4314,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>40</v>
@@ -4304,7 +4326,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>36</v>
@@ -4312,19 +4334,19 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C21" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D21" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="E21" s="4" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>36</v>
@@ -4332,19 +4354,19 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C22" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D22" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D22" s="4" t="n">
-        <v>3</v>
-      </c>
       <c r="E22" s="4" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>36</v>
@@ -4352,16 +4374,16 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C23" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4" t="n">
         <v>3</v>
-      </c>
-      <c r="D23" s="4" t="n">
-        <v>0</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>136</v>
@@ -4372,10 +4394,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>3</v>
@@ -4384,7 +4406,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>36</v>
@@ -4395,7 +4417,7 @@
         <v>53</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="C25" s="4" t="n">
         <v>3</v>
@@ -4415,7 +4437,7 @@
         <v>53</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>3</v>
@@ -4432,10 +4454,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C27" s="4" t="n">
         <v>3</v>
@@ -4455,7 +4477,7 @@
         <v>45</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>3</v>
@@ -4472,16 +4494,16 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C29" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D29" s="4" t="n">
         <v>0</v>
-      </c>
-      <c r="D29" s="4" t="n">
-        <v>3</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>139</v>
@@ -4495,13 +4517,13 @@
         <v>72</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="C30" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4" t="n">
         <v>3</v>
-      </c>
-      <c r="D30" s="4" t="n">
-        <v>0</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>139</v>
@@ -4512,10 +4534,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="C31" s="4" t="n">
         <v>3</v>
@@ -4532,16 +4554,16 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C32" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D32" s="4" t="n">
         <v>0</v>
-      </c>
-      <c r="D32" s="4" t="n">
-        <v>3</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>139</v>
@@ -4552,16 +4574,16 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="C33" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="4" t="n">
         <v>3</v>
-      </c>
-      <c r="D33" s="4" t="n">
-        <v>0</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>139</v>
@@ -4575,7 +4597,7 @@
         <v>40</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="C34" s="4" t="n">
         <v>3</v>
@@ -4592,16 +4614,16 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D35" s="4" t="n">
         <v>0</v>
-      </c>
-      <c r="D35" s="4" t="n">
-        <v>3</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>139</v>
@@ -4612,56 +4634,44 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="C36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D36" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="E36" s="4" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C37" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D37" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>68</v>
-      </c>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="C38" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D38" s="4" t="n">
         <v>0</v>
-      </c>
-      <c r="D38" s="4" t="n">
-        <v>3</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>127</v>
@@ -4672,10 +4682,10 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>3</v>
@@ -4692,7 +4702,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>63</v>
@@ -4704,7 +4714,7 @@
         <v>3</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>68</v>
@@ -4712,10 +4722,10 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>3</v>
@@ -4724,7 +4734,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>68</v>
@@ -4732,10 +4742,10 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C42" s="4" t="n">
         <v>0</v>
@@ -4744,7 +4754,7 @@
         <v>3</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>68</v>
@@ -4752,19 +4762,19 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="C43" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D43" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D43" s="4" t="n">
-        <v>3</v>
-      </c>
       <c r="E43" s="4" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>68</v>
@@ -4775,16 +4785,16 @@
         <v>70</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="C44" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D44" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="E44" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>68</v>
@@ -4792,19 +4802,19 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="C45" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D45" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="E45" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>68</v>
@@ -4812,10 +4822,10 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C46" s="4" t="n">
         <v>3</v>
@@ -4832,10 +4842,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C47" s="4" t="n">
         <v>3</v>
@@ -4855,13 +4865,13 @@
         <v>79</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="C48" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D48" s="4" t="n">
         <v>0</v>
-      </c>
-      <c r="D48" s="4" t="n">
-        <v>3</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>139</v>
@@ -4872,16 +4882,16 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C49" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D49" s="4" t="n">
         <v>0</v>
-      </c>
-      <c r="D49" s="4" t="n">
-        <v>3</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>139</v>
@@ -4892,16 +4902,16 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C50" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="4" t="n">
         <v>3</v>
-      </c>
-      <c r="D50" s="4" t="n">
-        <v>0</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>139</v>
@@ -4912,16 +4922,16 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C51" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="4" t="n">
         <v>3</v>
-      </c>
-      <c r="D51" s="4" t="n">
-        <v>0</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>139</v>
@@ -4932,10 +4942,10 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="C52" s="4" t="n">
         <v>3</v>
@@ -4952,10 +4962,10 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C53" s="4" t="n">
         <v>3</v>
@@ -4972,16 +4982,16 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="C54" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D54" s="4" t="n">
         <v>0</v>
-      </c>
-      <c r="D54" s="4" t="n">
-        <v>3</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>139</v>
@@ -4992,10 +5002,10 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C55" s="4" t="n">
         <v>3</v>
@@ -5007,6 +5017,46 @@
         <v>139</v>
       </c>
       <c r="F55" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D57" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F57" s="4" t="s">
         <v>68</v>
       </c>
     </row>
@@ -5034,10 +5084,10 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="21:21 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5251,10 +5301,10 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="21:21 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5542,10 +5592,10 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="21:21 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5821,13 +5871,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="21:21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5960,37 +6010,29 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>75</v>
-      </c>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="D12" s="4" t="n">
-        <v>250</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>36</v>
@@ -6004,49 +6046,49 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>233</v>
+        <v>136</v>
       </c>
       <c r="D14" s="4" t="n">
-        <v>500</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D15" s="4" t="n">
-        <v>375</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>127</v>
+        <v>234</v>
       </c>
       <c r="D16" s="4" t="n">
-        <v>125</v>
+        <v>375</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>36</v>
@@ -6060,7 +6102,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>36</v>
@@ -6074,7 +6116,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>36</v>
@@ -6088,91 +6130,83 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>50</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>234</v>
+        <v>139</v>
       </c>
       <c r="D21" s="4" t="n">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D22" s="4" t="n">
-        <v>125</v>
-      </c>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>136</v>
+        <v>234</v>
       </c>
       <c r="D23" s="4" t="n">
-        <v>125</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D24" s="4" t="n">
-        <v>65</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D25" s="4" t="n">
-        <v>65</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>68</v>
@@ -6186,7 +6220,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>68</v>
@@ -6200,43 +6234,71 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="D28" s="4" t="n">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>233</v>
+        <v>127</v>
       </c>
       <c r="D29" s="4" t="n">
-        <v>250</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="4" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D31" s="4" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D30" s="4" t="n">
+      <c r="D32" s="4" t="n">
         <v>25</v>
       </c>
     </row>
@@ -6263,11 +6325,11 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A50" activeCellId="1" sqref="21:21 A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -6300,14 +6362,14 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -6318,7 +6380,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B6" s="4"/>
@@ -6326,7 +6388,7 @@
       <c r="D6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -6337,7 +6399,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="4" t="s">
         <v>104</v>
       </c>
       <c r="C8" s="4"/>
@@ -6345,18 +6407,18 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="4" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B10" s="4"/>
@@ -6375,14 +6437,14 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -6420,7 +6482,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C17" s="4"/>
@@ -6471,13 +6533,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="4" t="s">
         <v>236</v>
       </c>
     </row>
@@ -6498,14 +6560,14 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="4" t="s">
         <v>102</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -6575,7 +6637,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B35" s="4"/>
@@ -6584,13 +6646,13 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="4" t="s">
         <v>236</v>
       </c>
     </row>
@@ -6611,7 +6673,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C39" s="4"/>
@@ -6656,7 +6718,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B44" s="4"/>
@@ -6665,18 +6727,18 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="4" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="4" t="s">
         <v>88</v>
       </c>
       <c r="C46" s="4"/>
@@ -7159,10 +7221,10 @@
   <dimension ref="A1:D262"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="21:21 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">

</xml_diff>

<commit_message>
fix: consistent sort on championship log
</commit_message>
<xml_diff>
--- a/tests/data_up_to_S2022T04/Torneo S2022T01 para publicar.xlsx
+++ b/tests/data_up_to_S2022T04/Torneo S2022T01 para publicar.xlsx
@@ -18,7 +18,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mi7rLkvb22G/rb0IWO4ltNpUzZClw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7migHTYlq/WDWDAePt6XZ4TR3cDjXw=="/>
     </ext>
   </extLst>
 </workbook>
@@ -15454,58 +15454,58 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="D7" s="4">
-        <v>250.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="D8" s="4">
-        <v>250.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="D9" s="4">
-        <v>500.0</v>
+        <v>250.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="D10" s="4">
-        <v>500.0</v>
+        <v>250.0</v>
       </c>
     </row>
     <row r="11">
@@ -15516,30 +15516,30 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>179</v>
+        <v>268</v>
       </c>
       <c r="D12" s="4">
-        <v>75.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>144</v>
+        <v>269</v>
       </c>
       <c r="D13" s="4">
-        <v>250.0</v>
+        <v>375.0</v>
       </c>
     </row>
     <row r="14">
@@ -15558,30 +15558,30 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>268</v>
+        <v>144</v>
       </c>
       <c r="D15" s="4">
-        <v>500.0</v>
+        <v>250.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>269</v>
+        <v>129</v>
       </c>
       <c r="D16" s="4">
-        <v>375.0</v>
+        <v>125.0</v>
       </c>
     </row>
     <row r="17">
@@ -15600,7 +15600,7 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>36</v>
@@ -15614,7 +15614,7 @@
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>36</v>
@@ -15628,19 +15628,19 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>129</v>
+        <v>179</v>
       </c>
       <c r="D20" s="4">
-        <v>125.0</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" s="4" t="s">
         <v>102</v>
       </c>
@@ -15654,7 +15654,7 @@
         <v>50.0</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -15662,35 +15662,35 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D23" s="4">
-        <v>190.0</v>
+        <v>250.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>144</v>
+        <v>269</v>
       </c>
       <c r="D24" s="4">
-        <v>125.0</v>
+        <v>190.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>68</v>
@@ -15704,21 +15704,21 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="D26" s="4">
-        <v>65.0</v>
+        <v>125.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>68</v>
@@ -15732,7 +15732,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>68</v>
@@ -15760,30 +15760,30 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="D30" s="4">
-        <v>40.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>268</v>
+        <v>179</v>
       </c>
       <c r="D31" s="4">
-        <v>250.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -15800,8 +15800,18 @@
         <v>25.0</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+    </row>
     <row r="35" ht="15.75" customHeight="1"/>
     <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1"/>
@@ -16768,6 +16778,8 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>

</xml_diff>

<commit_message>
tests: update xlsx to correct output and remove old figs
</commit_message>
<xml_diff>
--- a/tests/data_up_to_S2022T04/Torneo S2022T01 para publicar.xlsx
+++ b/tests/data_up_to_S2022T04/Torneo S2022T01 para publicar.xlsx
@@ -2310,22 +2310,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Velazquez, Marcelo (1460)</t>
+          <t>Perot, Alejandro (1634)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>591</t>
+          <t>417</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>-2</t>
+          <t>-4</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2352,22 +2352,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Perot, Alejandro (1634)</t>
+          <t>Velazquez, Marcelo (1460)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>417</t>
+          <t>591</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>-4</t>
+          <t>-2</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2730,22 +2730,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Larrosa, Jorge (516)</t>
+          <t>Godano, Franco (900)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>443</t>
+          <t>59</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>-2</t>
+          <t>-14</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2760,7 +2760,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2772,22 +2772,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Godano, Franco (900)</t>
+          <t>Larrosa, Jorge (516)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>443</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>-14</t>
+          <t>-2</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0.5</t>
         </is>
       </c>
     </row>
@@ -2814,37 +2814,37 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Larrosa, Jorge (516)</t>
+          <t>Bonelli, Marcos (959)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>649</t>
+          <t>206</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>-8</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>zona</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>segunda</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>zona</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>segunda</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>0.5</t>
         </is>
       </c>
     </row>
@@ -2898,22 +2898,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Bonelli, Marcos (959)</t>
+          <t>Larrosa, Jorge (516)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>206</t>
+          <t>649</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>-8</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2928,7 +2928,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0.5</t>
         </is>
       </c>
     </row>
@@ -2940,22 +2940,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Goy, Gerardo (848)</t>
+          <t>Escudero, Martin (1063)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>443</t>
+          <t>228</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>-2</t>
+          <t>-8</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2970,7 +2970,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2982,22 +2982,22 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Escudero, Martin (1063)</t>
+          <t>Goy, Gerardo (848)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>228</t>
+          <t>443</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>-8</t>
+          <t>-2</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3012,7 +3012,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0.5</t>
         </is>
       </c>
     </row>
@@ -3150,37 +3150,37 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Prettis, Juan (568)</t>
+          <t>Levin, Raul (988)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>772</t>
+          <t>352</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>-6</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>zona</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>segunda</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>zona</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>segunda</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>0.5</t>
         </is>
       </c>
     </row>
@@ -3192,22 +3192,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Levin, Raul (988)</t>
+          <t>Prettis, Juan (568)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>352</t>
+          <t>772</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>-6</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3222,7 +3222,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0.5</t>
         </is>
       </c>
     </row>
@@ -3570,12 +3570,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Prettis, Juan (568)</t>
+          <t>Godano, Lucas (612)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>316</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3612,12 +3612,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Godano, Lucas (612)</t>
+          <t>Prettis, Juan (568)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>360</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -4390,7 +4390,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Velazquez, Marcelo</t>
+          <t>Perot, Alejandro</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Perot, Alejandro</t>
+          <t>Velazquez, Marcelo</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -4698,7 +4698,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Larrosa, Jorge</t>
+          <t>Bonelli, Marcos</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -4754,7 +4754,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Bonelli, Marcos</t>
+          <t>Larrosa, Jorge</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -4782,7 +4782,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Goy, Gerardo</t>
+          <t>Escudero, Martin</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -4810,7 +4810,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Escudero, Martin</t>
+          <t>Goy, Gerardo</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -4950,7 +4950,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Prettis, Juan</t>
+          <t>Levin, Raul</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -4978,7 +4978,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Levin, Raul</t>
+          <t>Prettis, Juan</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -5258,7 +5258,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Prettis, Juan</t>
+          <t>Godano, Lucas</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -5286,7 +5286,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Godano, Lucas</t>
+          <t>Prettis, Juan</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -5342,14 +5342,14 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Suarez, Milton</t>
+          <t>Jaime, Gerardo</t>
         </is>
       </c>
       <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
         <v>3</v>
-      </c>
-      <c r="D49" t="n">
-        <v>0</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -5370,14 +5370,14 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Jaime, Gerardo</t>
+          <t>Suarez, Milton</t>
         </is>
       </c>
       <c r="C50" t="n">
+        <v>3</v>
+      </c>
+      <c r="D50" t="n">
         <v>0</v>
-      </c>
-      <c r="D50" t="n">
-        <v>3</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -5538,14 +5538,14 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Jaime, Gerardo</t>
+          <t>Escalante, Samuel</t>
         </is>
       </c>
       <c r="C56" t="n">
+        <v>3</v>
+      </c>
+      <c r="D56" t="n">
         <v>0</v>
-      </c>
-      <c r="D56" t="n">
-        <v>3</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -5566,14 +5566,14 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Escalante, Samuel</t>
+          <t>Jaime, Gerardo</t>
         </is>
       </c>
       <c r="C57" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" t="n">
         <v>3</v>
-      </c>
-      <c r="D57" t="n">
-        <v>0</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -8331,12 +8331,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Nowotny, Martin</t>
+          <t>Dupertuis, Gaston</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Libertador San Martin</t>
+          <t>Parana</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Aspatem</t>
         </is>
       </c>
     </row>
@@ -8346,17 +8351,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Dupertuis, Gaston</t>
+          <t>Nowotny, Martin</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Parana</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Aspatem</t>
+          <t>Libertador San Martin</t>
         </is>
       </c>
     </row>
@@ -8426,7 +8426,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>La Barba, Pablo</t>
+          <t>Aguirre, German</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -8446,7 +8446,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Aguirre, German</t>
+          <t>La Barba, Pablo</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -9046,7 +9046,17 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Sueldo, Pablo</t>
+          <t>Sartor, Yemel</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Avellaneda</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>ATMAR</t>
         </is>
       </c>
     </row>
@@ -9056,17 +9066,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Sartor, Yemel</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Avellaneda</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>ATMAR</t>
+          <t>Sueldo, Pablo</t>
         </is>
       </c>
     </row>
@@ -9281,17 +9281,17 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Maerker, Shion</t>
+          <t>Becker, Fernando</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Libertador San Martin</t>
+          <t>Parana</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>CRL</t>
+          <t>Aspatem</t>
         </is>
       </c>
     </row>
@@ -9301,17 +9301,17 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Becker, Fernando</t>
+          <t>Maerker, Shion</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Parana</t>
+          <t>Libertador San Martin</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Aspatem</t>
+          <t>CRL</t>
         </is>
       </c>
     </row>
@@ -9356,17 +9356,17 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Chiara, Lucio</t>
+          <t>Campos, Dario</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Parana</t>
+          <t>Santa Fe</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Aspatem</t>
+          <t>Atemeli</t>
         </is>
       </c>
     </row>
@@ -9376,17 +9376,17 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Campos, Dario</t>
+          <t>Chiara, Lucio</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Santa Fe</t>
+          <t>Parana</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Atemeli</t>
+          <t>Aspatem</t>
         </is>
       </c>
     </row>
@@ -9396,7 +9396,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Lerch, Juan Carlos</t>
+          <t>Gimenez, Maximo</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -9406,7 +9406,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Tiro Federal</t>
+          <t>Aspatem</t>
         </is>
       </c>
     </row>
@@ -9416,7 +9416,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Gimenez, Maximo</t>
+          <t>Lerch, Juan Carlos</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -9426,7 +9426,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Aspatem</t>
+          <t>Tiro Federal</t>
         </is>
       </c>
     </row>
@@ -9776,12 +9776,17 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Mendieta, Elias</t>
+          <t>Arrieta, Maximiliano</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Santa Fe</t>
+          <t>Libertador San Martin</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>CRL</t>
         </is>
       </c>
     </row>
@@ -9791,17 +9796,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Badano, Pablo</t>
+          <t>Asenie, Santiago</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Parana</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>Aspatem</t>
+          <t>Libertador San Martin</t>
         </is>
       </c>
     </row>
@@ -9811,12 +9811,17 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Asenie, Santiago</t>
+          <t>Badano, Pablo</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Libertador San Martin</t>
+          <t>Parana</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Aspatem</t>
         </is>
       </c>
     </row>
@@ -9846,17 +9851,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Presel, Raul</t>
+          <t>Mendieta, Elias</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Parana</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>Aspatem</t>
+          <t>Santa Fe</t>
         </is>
       </c>
     </row>
@@ -9866,17 +9866,17 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Arrieta, Maximiliano</t>
+          <t>Presel, Raul</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Libertador San Martin</t>
+          <t>Parana</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>CRL</t>
+          <t>Aspatem</t>
         </is>
       </c>
     </row>
@@ -10871,7 +10871,17 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Martinez, Dylan</t>
+          <t>Aguirre, Gabriel</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Parana</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Aspatem</t>
         </is>
       </c>
     </row>
@@ -10881,17 +10891,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Aguirre, Gabriel</t>
-        </is>
-      </c>
-      <c r="C170" t="inlineStr">
-        <is>
-          <t>Parana</t>
-        </is>
-      </c>
-      <c r="D170" t="inlineStr">
-        <is>
-          <t>Aspatem</t>
+          <t>Martinez, Dylan</t>
         </is>
       </c>
     </row>
@@ -10971,17 +10971,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Werner, Graciela</t>
-        </is>
-      </c>
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>Parana</t>
-        </is>
-      </c>
-      <c r="D175" t="inlineStr">
-        <is>
-          <t>Aspatem</t>
+          <t>Rodriguez Alarcon Emiliano</t>
         </is>
       </c>
     </row>
@@ -10991,7 +10981,17 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Rodriguez Alarcon Emiliano</t>
+          <t>Werner, Graciela</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Parana</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Aspatem</t>
         </is>
       </c>
     </row>
@@ -11001,7 +11001,17 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Mir, Tomas</t>
+          <t>Javita, Luis</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Libertador San Martin</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>CRL</t>
         </is>
       </c>
     </row>
@@ -11021,17 +11031,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Javita, Luis</t>
-        </is>
-      </c>
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>Libertador San Martin</t>
-        </is>
-      </c>
-      <c r="D179" t="inlineStr">
-        <is>
-          <t>CRL</t>
+          <t>Mir, Tomas</t>
         </is>
       </c>
     </row>
@@ -11156,7 +11156,17 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Michea, Ignacio</t>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Libertador San Martin</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>CRL</t>
         </is>
       </c>
     </row>
@@ -11166,17 +11176,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Jose</t>
-        </is>
-      </c>
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>Libertador San Martin</t>
-        </is>
-      </c>
-      <c r="D190" t="inlineStr">
-        <is>
-          <t>CRL</t>
+          <t>Michea, Ignacio</t>
         </is>
       </c>
     </row>
@@ -11221,17 +11221,17 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Portillo, Lucas</t>
+          <t>Arrieta, Matias</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Esperanza</t>
+          <t>Libertador San Martin</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>ATME</t>
+          <t>CRL</t>
         </is>
       </c>
     </row>
@@ -11256,17 +11256,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Arrieta, Matias</t>
-        </is>
-      </c>
-      <c r="C196" t="inlineStr">
-        <is>
-          <t>Libertador San Martin</t>
-        </is>
-      </c>
-      <c r="D196" t="inlineStr">
-        <is>
-          <t>CRL</t>
+          <t>Muller, Tomas</t>
         </is>
       </c>
     </row>
@@ -11276,7 +11266,17 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Muller, Tomas</t>
+          <t>Portillo, Lucas</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Esperanza</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>ATME</t>
         </is>
       </c>
     </row>
@@ -11336,17 +11336,17 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Pillac, Juan Pablo</t>
+          <t>Comas, Javier</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Libertador San Martin</t>
+          <t>Parana</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>CRL</t>
+          <t>Aspatem</t>
         </is>
       </c>
     </row>
@@ -11356,17 +11356,17 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Comas, Javier</t>
+          <t>Pillac, Juan Pablo</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>Parana</t>
+          <t>Libertador San Martin</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>Aspatem</t>
+          <t>CRL</t>
         </is>
       </c>
     </row>
@@ -11496,17 +11496,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Vergara, Gustavo</t>
-        </is>
-      </c>
-      <c r="C212" t="inlineStr">
-        <is>
-          <t>Parana</t>
-        </is>
-      </c>
-      <c r="D212" t="inlineStr">
-        <is>
-          <t>Tiro Federal</t>
+          <t>Godano, Lucas</t>
         </is>
       </c>
     </row>
@@ -11516,7 +11506,17 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Godano, Lucas</t>
+          <t>Vergara, Gustavo</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Parana</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>Tiro Federal</t>
         </is>
       </c>
     </row>
@@ -11701,7 +11701,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Musuruana, Francisco</t>
+          <t>Escalante, Samuel</t>
         </is>
       </c>
     </row>
@@ -11711,7 +11711,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Escalante, Samuel</t>
+          <t>Musuruana, Francisco</t>
         </is>
       </c>
     </row>
@@ -11926,7 +11926,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Ferrero, Alejandro</t>
+          <t>Antunez, Pablo</t>
         </is>
       </c>
     </row>
@@ -11936,7 +11936,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Antunez, Pablo</t>
+          <t>Ferrero, Alejandro</t>
         </is>
       </c>
     </row>
@@ -11956,7 +11956,17 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Velazquez, Pedro</t>
+          <t>Lell, Claudia</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>Parana</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>Tiro Federal</t>
         </is>
       </c>
     </row>
@@ -11966,17 +11976,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Lell, Claudia</t>
-        </is>
-      </c>
-      <c r="C245" t="inlineStr">
-        <is>
-          <t>Parana</t>
-        </is>
-      </c>
-      <c r="D245" t="inlineStr">
-        <is>
-          <t>Tiro Federal</t>
+          <t>Velazquez, Pedro</t>
         </is>
       </c>
     </row>
@@ -12066,7 +12066,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Bertoli, Maximiliano</t>
+          <t>Bertoli, Julian</t>
         </is>
       </c>
     </row>
@@ -12076,7 +12076,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Bertoli, Julian</t>
+          <t>Bertoli, Maximiliano</t>
         </is>
       </c>
     </row>
@@ -12086,17 +12086,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Seib, Silvia</t>
-        </is>
-      </c>
-      <c r="C254" t="inlineStr">
-        <is>
-          <t>Parana</t>
-        </is>
-      </c>
-      <c r="D254" t="inlineStr">
-        <is>
-          <t>Aspatem</t>
+          <t>Macor, Mateo</t>
         </is>
       </c>
     </row>
@@ -12106,7 +12096,17 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Macor, Mateo</t>
+          <t>Seib, Silvia</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Parana</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Aspatem</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing publish reference xlsx files for test
</commit_message>
<xml_diff>
--- a/tests/data_up_to_S2022T04/Torneo S2022T01 para publicar.xlsx
+++ b/tests/data_up_to_S2022T04/Torneo S2022T01 para publicar.xlsx
@@ -1696,8 +1696,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4069,8 +4069,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5589,8 +5589,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5878,8 +5878,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6273,8 +6273,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6653,8 +6653,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -7255,8 +7255,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>